<commit_message>
Removed not needed files and changes on availability
</commit_message>
<xml_diff>
--- a/playwright/testData.xlsx
+++ b/playwright/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquintero\proyectos\automation-ssci\playwright\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquintero\proyectos\automation-booking\playwright\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A54BA0-854D-4269-A0BD-DB0775D8A3B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CC8D9-184A-437A-B1DD-90BC63989C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{A75A5039-BE99-42B9-9564-A3A62C427F9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{A75A5039-BE99-42B9-9564-A3A62C427F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Server" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>TestName</t>
   </si>
@@ -42,18 +42,45 @@
     <t>language</t>
   </si>
   <si>
+    <t>nbAdults</t>
+  </si>
+  <si>
+    <t>nbChildren</t>
+  </si>
+  <si>
+    <t>nbInfants</t>
+  </si>
+  <si>
     <t>pointOfSale</t>
   </si>
   <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
     <t>trace</t>
   </si>
   <si>
+    <t>tripType</t>
+  </si>
+  <si>
+    <t>BOG</t>
+  </si>
+  <si>
+    <t>MDE</t>
+  </si>
+  <si>
     <t>all</t>
   </si>
   <si>
     <t>EU</t>
   </si>
   <si>
+    <t>round-trip</t>
+  </si>
+  <si>
     <t>https://uat.digital.airline.amadeus.com/av/booking/avail</t>
   </si>
   <si>
@@ -61,6 +88,9 @@
   </si>
   <si>
     <t>Release_UAT</t>
+  </si>
+  <si>
+    <t>https://uat.digital.airline.amadeus.com/av/release-booking/avail</t>
   </si>
   <si>
     <r>
@@ -83,6 +113,15 @@
     <t>Production</t>
   </si>
   <si>
+    <t>departureDate</t>
+  </si>
+  <si>
+    <t>returnDate</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
     <t>creditCardType</t>
   </si>
   <si>
@@ -98,9 +137,21 @@
     <t>cardInfo</t>
   </si>
   <si>
+    <t>one-way</t>
+  </si>
+  <si>
+    <t>Amex</t>
+  </si>
+  <si>
     <t>377813402429063,03/25,3551</t>
   </si>
   <si>
+    <t>VC_Test_01_availability_screen</t>
+  </si>
+  <si>
+    <t>VC_Test_01_passenger_screen</t>
+  </si>
+  <si>
     <t>Demo</t>
   </si>
   <si>
@@ -110,9 +161,18 @@
     <t>PT</t>
   </si>
   <si>
+    <t>fareInBound</t>
+  </si>
+  <si>
+    <t>fareOutBound</t>
+  </si>
+  <si>
     <t>Carry-on</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>LifeMiles</t>
   </si>
   <si>
@@ -125,18 +185,54 @@
     <t>SpecialAssistance</t>
   </si>
   <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>PTY</t>
+  </si>
+  <si>
+    <t>LIM</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>SportEquipment</t>
   </si>
   <si>
     <t>Insurance</t>
   </si>
   <si>
+    <t>PSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">BuyExtraBaggage </t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>OnSite</t>
+  </si>
+  <si>
     <t>AuthorizationID</t>
   </si>
   <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>AditionalData</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>cardHolderName</t>
   </si>
   <si>
@@ -155,12 +251,45 @@
     <t>Approved</t>
   </si>
   <si>
+    <t>accept@accept.com</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Street 85 #25-30$</t>
+  </si>
+  <si>
+    <t>Test_05_PT_BR_OW_BookingPNR</t>
+  </si>
+  <si>
+    <t>Test_01_PT_EU_RT_BookingPNR</t>
+  </si>
+  <si>
+    <t>Test_02_EN_US_RT_BookingPNR</t>
+  </si>
+  <si>
+    <t>Test_03_SP_CO_RT_BookingPNR</t>
+  </si>
+  <si>
+    <t>Test_04_SP_CO_OW_BookingPNR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
     <t>Seat</t>
   </si>
   <si>
+    <t>Covid</t>
+  </si>
+  <si>
     <t>useHPP</t>
   </si>
   <si>
+    <t>DFW</t>
+  </si>
+  <si>
     <t>PR</t>
   </si>
   <si>
@@ -170,31 +299,19 @@
     <t>WEBB2C</t>
   </si>
   <si>
-    <t>https://dev.digital.airline.amadeus.com/av/booking-15-6-5-pr-597/avail</t>
-  </si>
-  <si>
-    <t>https://uat.digital.airline.amadeus.com/av/release-ssci/identification?identifier=2PLNWG&amp;lang=ES&amp;lastName=Sosa&amp;overrides=%7B%22useHPP%22%3A%22true%22%7D&amp;pointOfSale=CO</t>
-  </si>
-  <si>
-    <t>https://uat.digital.airline.amadeus.com/av/release-ssci/</t>
-  </si>
-  <si>
-    <t>pnr</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>Sosa</t>
-  </si>
-  <si>
-    <t>Test_01_PT_EU_RT_SSCI</t>
-  </si>
-  <si>
-    <t>https://uat.digital.airline.amadeus.com/av/release-ssci/?identification?identifier=2PLNWG&amp;lang=PT&amp;lastName=Sosa&amp;pointOfSale=EU&amp;trace=all&amp;overrides=%7B%22isExternalScriptsActivated%22%3A%22false%22%2C%22useHPP%22%3A%22true%22%7D</t>
-  </si>
-  <si>
-    <t>3DFCIK</t>
+    <t>L</t>
+  </si>
+  <si>
+    <t>https://dev.digital.airline.amadeus.com/av/booking-15-6-8-pr-724/avail</t>
+  </si>
+  <si>
+    <t>PSO</t>
+  </si>
+  <si>
+    <t>https://dev.digital.airline.amadeus.com/av/booking-16-6/avail?departureDate=2022-09-19&amp;from=BOG&amp;language=ES&amp;nbAdults=1&amp;nbAnimals=0&amp;nbChildren=0&amp;nbInfants=0&amp;platform=WEBB2C&amp;pointOfSale=EU&amp;returnDate=2022-09-26&amp;to=MDE&amp;tripType=round-trip</t>
+  </si>
+  <si>
+    <t>https://dev.digital.airline.amadeus.com/av/booking-16-6/avail</t>
   </si>
 </sst>
 </file>
@@ -246,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,21 +422,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -631,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207235F5-B287-439B-BA60-715477EC9E77}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,62 +779,68 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3"/>
+      <c r="B6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" s="6"/>
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="5"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="2"/>
@@ -706,12 +848,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{A6E0811F-BDF1-4E7D-B7A8-CFF0EF799DC3}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{0958F228-44CD-4D2A-81C0-4C91E2E514CC}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{8B69920D-D9E3-40CA-A8B0-EAC3021BD195}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{AD61F9DA-8A2C-46B0-89DE-BC952E38286B}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{7CD84B30-BF5F-4607-A5AC-2B64EC67B102}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{8CD33CA3-B113-433E-AF0A-144133F18906}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;KFF8C00CONFIDENTIAL &amp; RESTRICTED&amp;1#</oddHeader>
   </headerFooter>
@@ -720,184 +861,700 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045B99D3-EDEC-4FE9-AF92-0244EBD3F8CC}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AL8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75">
+    <row r="1" spans="1:38" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" s="9" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="11">
+        <f ca="1">+(((TODAY()+51)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1667433600000</v>
+      </c>
+      <c r="F2" s="11">
+        <f ca="1">+(((TODAY()+55)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1667779200000</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="AB2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" s="12"/>
+      <c r="AL2" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" s="9" customFormat="1">
+      <c r="A3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="11">
+        <f ca="1">+(((TODAY()+68)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1668902400000</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10">
+        <v>2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>123456</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH3" s="9">
+        <v>987654321</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ3" s="9">
+        <v>35801</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" s="9" customFormat="1">
+      <c r="A4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="11">
+        <f ca="1">+(((TODAY()+17)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1664496000000</v>
+      </c>
+      <c r="F4" s="11">
+        <f ca="1">+(((TODAY()+28)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1665446400000</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2</v>
+      </c>
+      <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" s="9" customFormat="1">
+      <c r="A5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11">
+        <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1663632000000</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>321321</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38">
+      <c r="A6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="11">
+        <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1663632000000</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>123456</v>
+      </c>
+      <c r="AG6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH6" s="9">
+        <v>987654321</v>
+      </c>
+      <c r="AI6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ6" s="9">
+        <v>35801</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5">
+        <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1663459200000</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Z7" s="4"/>
+    </row>
+    <row r="8" spans="1:38">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5">
+        <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
+        <v>1663459200000</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" s="5" customFormat="1">
-      <c r="A2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="6"/>
-      <c r="AB2" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z8" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="AG3" r:id="rId1" xr:uid="{ADE3AF93-4FF1-43B6-982A-173B164DAE84}"/>
+    <hyperlink ref="AG6" r:id="rId2" xr:uid="{D90988AC-DD61-4558-9FFF-0715659DF942}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;KFF8C00CONFIDENTIAL &amp; RESTRICTED&amp;1#</oddHeader>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="E5" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change in ancillaries page
</commit_message>
<xml_diff>
--- a/playwright/testData.xlsx
+++ b/playwright/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquintero\proyectos\automation-booking\playwright\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CC8D9-184A-437A-B1DD-90BC63989C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CC7D48-C4E2-44B3-ACF6-D0C95F6ACA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{A75A5039-BE99-42B9-9564-A3A62C427F9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{A75A5039-BE99-42B9-9564-A3A62C427F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Server" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>TestName</t>
   </si>
@@ -209,9 +209,6 @@
     <t>PSE</t>
   </si>
   <si>
-    <t xml:space="preserve">BuyExtraBaggage </t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -312,6 +309,15 @@
   </si>
   <si>
     <t>https://dev.digital.airline.amadeus.com/av/booking-16-6/avail</t>
+  </si>
+  <si>
+    <t>cardName</t>
+  </si>
+  <si>
+    <t>Approved Approved</t>
+  </si>
+  <si>
+    <t>BuyExtraBaggage</t>
   </si>
 </sst>
 </file>
@@ -767,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207235F5-B287-439B-BA60-715477EC9E77}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -798,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -811,10 +817,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -824,7 +830,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -861,10 +867,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045B99D3-EDEC-4FE9-AF92-0244EBD3F8CC}">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AM8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -898,17 +904,18 @@
     <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.75">
+    <row r="1" spans="1:39" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,13 +944,13 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
@@ -961,7 +968,7 @@
         <v>40</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>42</v>
@@ -976,10 +983,10 @@
         <v>52</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>20</v>
@@ -994,39 +1001,42 @@
         <v>29</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AD1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" s="9" customFormat="1">
+      <c r="AM1" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" s="9" customFormat="1">
       <c r="A2" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>37</v>
@@ -1039,11 +1049,11 @@
       </c>
       <c r="E2" s="11">
         <f ca="1">+(((TODAY()+51)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1667433600000</v>
+        <v>1667865600000</v>
       </c>
       <c r="F2" s="11">
         <f ca="1">+(((TODAY()+55)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1667779200000</v>
+        <v>1668211200000</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -1068,10 +1078,10 @@
         <v>14</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>41</v>
@@ -1099,19 +1109,22 @@
         <v>32</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="12"/>
-      <c r="AL2" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" s="9" customFormat="1">
+        <v>66</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH2" s="12"/>
+      <c r="AM2" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" s="9" customFormat="1">
       <c r="A3" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>24</v>
@@ -1120,11 +1133,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="11">
         <f ca="1">+(((TODAY()+68)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1668902400000</v>
+        <v>1669334400000</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="10">
@@ -1137,10 +1150,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" s="10" t="b">
         <v>0</v>
@@ -1152,10 +1165,10 @@
         <v>30</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
@@ -1177,37 +1190,37 @@
       <c r="AB3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AD3" s="9" t="s">
+      <c r="AE3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG3" s="9">
+        <v>123456</v>
+      </c>
+      <c r="AH3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AE3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF3" s="9">
-        <v>123456</v>
-      </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AI3" s="9">
+        <v>987654321</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AH3" s="9">
-        <v>987654321</v>
-      </c>
-      <c r="AI3" s="9" t="s">
+      <c r="AK3" s="9">
+        <v>35801</v>
+      </c>
+      <c r="AL3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AJ3" s="9">
-        <v>35801</v>
-      </c>
-      <c r="AK3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL3" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" s="9" customFormat="1">
+      <c r="AM3" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" s="9" customFormat="1">
       <c r="A4" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>46</v>
@@ -1216,15 +1229,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="11">
         <f ca="1">+(((TODAY()+17)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1664496000000</v>
+        <v>1664928000000</v>
       </c>
       <c r="F4" s="11">
         <f ca="1">+(((TODAY()+28)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1665446400000</v>
+        <v>1665878400000</v>
       </c>
       <c r="G4" s="10">
         <v>2</v>
@@ -1249,10 +1262,10 @@
         <v>14</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -1266,15 +1279,15 @@
         <v>17</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" s="9" customFormat="1">
+        <v>55</v>
+      </c>
+      <c r="AM4" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" s="9" customFormat="1">
       <c r="A5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>46</v>
@@ -1287,7 +1300,7 @@
       </c>
       <c r="E5" s="11">
         <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663632000000</v>
+        <v>1664064000000</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="10">
@@ -1339,13 +1352,13 @@
       <c r="AC5" s="9">
         <v>321321</v>
       </c>
-      <c r="AL5" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38">
+      <c r="AM5" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
       <c r="A6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>37</v>
@@ -1354,11 +1367,11 @@
         <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="11">
         <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663632000000</v>
+        <v>1664064000000</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="10">
@@ -1371,10 +1384,10 @@
         <v>1</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L6" s="10" t="b">
         <v>1</v>
@@ -1408,35 +1421,36 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="9" t="s">
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG6" s="9">
+        <v>123456</v>
+      </c>
+      <c r="AH6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AE6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF6" s="9">
-        <v>123456</v>
-      </c>
-      <c r="AG6" s="12" t="s">
+      <c r="AI6" s="9">
+        <v>987654321</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AH6" s="9">
-        <v>987654321</v>
-      </c>
-      <c r="AI6" s="9" t="s">
+      <c r="AK6" s="9">
+        <v>35801</v>
+      </c>
+      <c r="AL6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AJ6" s="9">
-        <v>35801</v>
-      </c>
-      <c r="AK6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL6" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38">
+      <c r="AM6" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1465,7 @@
       </c>
       <c r="E7" s="5">
         <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663459200000</v>
+        <v>1663891200000</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="4">
@@ -1489,7 +1503,7 @@
       </c>
       <c r="Z7" s="4"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1504,7 +1518,7 @@
       </c>
       <c r="E8" s="5">
         <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663459200000</v>
+        <v>1663891200000</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="4">
@@ -1545,8 +1559,8 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AG3" r:id="rId1" xr:uid="{ADE3AF93-4FF1-43B6-982A-173B164DAE84}"/>
-    <hyperlink ref="AG6" r:id="rId2" xr:uid="{D90988AC-DD61-4558-9FFF-0715659DF942}"/>
+    <hyperlink ref="AH3" r:id="rId1" xr:uid="{ADE3AF93-4FF1-43B6-982A-173B164DAE84}"/>
+    <hyperlink ref="AH6" r:id="rId2" xr:uid="{D90988AC-DD61-4558-9FFF-0715659DF942}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>

</xml_diff>

<commit_message>
Fix the mobile flow
</commit_message>
<xml_diff>
--- a/playwright/testData.xlsx
+++ b/playwright/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquintero\proyectos\automation-booking\playwright\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CC7D48-C4E2-44B3-ACF6-D0C95F6ACA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C638F1-7422-4B07-81BC-81241B645DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{A75A5039-BE99-42B9-9564-A3A62C427F9E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
   <si>
     <t>TestName</t>
   </si>
@@ -302,9 +302,6 @@
     <t>https://dev.digital.airline.amadeus.com/av/booking-15-6-8-pr-724/avail</t>
   </si>
   <si>
-    <t>PSO</t>
-  </si>
-  <si>
     <t>https://dev.digital.airline.amadeus.com/av/booking-16-6/avail?departureDate=2022-09-19&amp;from=BOG&amp;language=ES&amp;nbAdults=1&amp;nbAnimals=0&amp;nbChildren=0&amp;nbInfants=0&amp;platform=WEBB2C&amp;pointOfSale=EU&amp;returnDate=2022-09-26&amp;to=MDE&amp;tripType=round-trip</t>
   </si>
   <si>
@@ -318,6 +315,12 @@
   </si>
   <si>
     <t>BuyExtraBaggage</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>MAD</t>
   </si>
 </sst>
 </file>
@@ -804,7 +807,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -830,7 +833,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -869,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045B99D3-EDEC-4FE9-AF92-0244EBD3F8CC}">
   <dimension ref="A1:AM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -968,7 +971,7 @@
         <v>40</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>42</v>
@@ -1004,7 +1007,7 @@
         <v>56</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AE1" s="8" t="s">
         <v>61</v>
@@ -1049,11 +1052,11 @@
       </c>
       <c r="E2" s="11">
         <f ca="1">+(((TODAY()+51)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1667865600000</v>
+        <v>1668211200000</v>
       </c>
       <c r="F2" s="11">
         <f ca="1">+(((TODAY()+55)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1668211200000</v>
+        <v>1668556800000</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -1109,7 +1112,7 @@
         <v>32</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE2" s="9" t="s">
         <v>66</v>
@@ -1137,7 +1140,7 @@
       </c>
       <c r="E3" s="11">
         <f ca="1">+(((TODAY()+68)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1669334400000</v>
+        <v>1669680000000</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="10">
@@ -1229,15 +1232,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E4" s="11">
         <f ca="1">+(((TODAY()+17)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1664928000000</v>
+        <v>1665273600000</v>
       </c>
       <c r="F4" s="11">
         <f ca="1">+(((TODAY()+28)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1665878400000</v>
+        <v>1666224000000</v>
       </c>
       <c r="G4" s="10">
         <v>2</v>
@@ -1253,7 +1256,7 @@
         <v>49</v>
       </c>
       <c r="L4" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>12</v>
@@ -1265,7 +1268,7 @@
         <v>54</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -1300,7 +1303,7 @@
       </c>
       <c r="E5" s="11">
         <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1664064000000</v>
+        <v>1664409600000</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="10">
@@ -1371,7 +1374,7 @@
       </c>
       <c r="E6" s="11">
         <f ca="1">+(((TODAY()+7)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1664064000000</v>
+        <v>1664409600000</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="10">
@@ -1465,7 +1468,7 @@
       </c>
       <c r="E7" s="5">
         <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663891200000</v>
+        <v>1664236800000</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="4">
@@ -1518,7 +1521,7 @@
       </c>
       <c r="E8" s="5">
         <f ca="1">+(((TODAY()+5)-DATE(1970,1,1))*86400000)+86400000</f>
-        <v>1663891200000</v>
+        <v>1664236800000</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="4">

</xml_diff>